<commit_message>
add cellFormat dateShort, dateLarge, start work on Time
</commit_message>
<xml_diff>
--- a/Excelam.Tests/Files/Cells/GetManyCellTypes.xlsx
+++ b/Excelam.Tests/Files/Cells/GetManyCellTypes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a990f455bb745add/ProjetsDev/70-yvlawy/Excelam/Dev/ExcelamSol/Excelam.Tests/Files/Cells/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="97" documentId="11_F25DC773A252ABDACC1048F0A91D62385BDE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{311E710C-F943-4A84-A3A7-B650451203EE}"/>
+  <xr:revisionPtr revIDLastSave="101" documentId="11_F25DC773A252ABDACC1048F0A91D62385BDE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E3FEF3E4-552D-43F0-B0CF-1268EE8B692F}"/>
   <bookViews>
-    <workbookView xWindow="2700" yWindow="120" windowWidth="16365" windowHeight="10800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="360" yWindow="120" windowWidth="18945" windowHeight="10800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>bonjour</t>
   </si>
@@ -110,7 +110,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="7">
+  <numFmts count="8">
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="0.000%"/>
@@ -118,6 +118,7 @@
     <numFmt numFmtId="167" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
     <numFmt numFmtId="168" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
     <numFmt numFmtId="169" formatCode="#,##0.00\ &quot;€&quot;"/>
+    <numFmt numFmtId="171" formatCode="[$$-409]#,##0.00"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -175,7 +176,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -195,6 +196,7 @@
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -475,10 +477,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -643,6 +645,14 @@
         <v>88.22</v>
       </c>
     </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23" s="19">
+        <v>91.25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>